<commit_message>
Update LMS scenarios excel files
</commit_message>
<xml_diff>
--- a/Excel_files_for_MISSAR/Prospective_scenarios/2014_q4_start/Historical_graphs_ages_16_69/Economic_scenarios_representation_dec_2019.xlsx
+++ b/Excel_files_for_MISSAR/Prospective_scenarios/2014_q4_start/Historical_graphs_ages_16_69/Economic_scenarios_representation_dec_2019.xlsx
@@ -829,7 +829,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart51.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -840,10 +840,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0524939822416349"/>
-          <c:y val="0.0202788339670469"/>
-          <c:w val="0.917473019719118"/>
-          <c:h val="0.625608698552465"/>
+          <c:x val="0.0524890913144568"/>
+          <c:y val="0.0202795103565592"/>
+          <c:w val="0.917460266904481"/>
+          <c:h val="0.625596210933591"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -14165,6 +14165,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="261"/>
+                <c:pt idx="179">
+                  <c:v>1.00000000001714</c:v>
+                </c:pt>
                 <c:pt idx="182">
                   <c:v>0.0807060966628571</c:v>
                 </c:pt>
@@ -16390,10 +16393,10 @@
                   <c:v>0.0807060966628571</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>0.0802182917848084</c:v>
+                  <c:v>0.0802182917848083</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>0.0797304869067596</c:v>
+                  <c:v>0.0797304869067595</c:v>
                 </c:pt>
                 <c:pt idx="185">
                   <c:v>0.0792426820287108</c:v>
@@ -16408,7 +16411,7 @@
                   <c:v>0.0777792673945644</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>0.0772914625165157</c:v>
+                  <c:v>0.0772914625165156</c:v>
                 </c:pt>
                 <c:pt idx="190">
                   <c:v>0.0768036576384669</c:v>
@@ -16423,10 +16426,10 @@
                   <c:v>0.0753402430043205</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>0.0748524381262718</c:v>
+                  <c:v>0.0748524381262717</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>0.074364633248223</c:v>
+                  <c:v>0.0743646332482229</c:v>
                 </c:pt>
                 <c:pt idx="196">
                   <c:v>0.0738768283701742</c:v>
@@ -16438,10 +16441,10 @@
                   <c:v>0.0729012186140766</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>0.0724134137360279</c:v>
+                  <c:v>0.0724134137360278</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>0.0719256088579791</c:v>
+                  <c:v>0.071925608857979</c:v>
                 </c:pt>
                 <c:pt idx="201">
                   <c:v>0.0714378039799303</c:v>
@@ -16453,10 +16456,10 @@
                   <c:v>0.0704621942238327</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>0.069974389345784</c:v>
+                  <c:v>0.0699743893457839</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>0.0694865844677352</c:v>
+                  <c:v>0.0694865844677351</c:v>
                 </c:pt>
                 <c:pt idx="206">
                   <c:v>0.0689987795896864</c:v>
@@ -16471,7 +16474,7 @@
                   <c:v>0.06753536495554</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>0.0670475600774913</c:v>
+                  <c:v>0.0670475600774912</c:v>
                 </c:pt>
                 <c:pt idx="211">
                   <c:v>0.0665597551994425</c:v>
@@ -16486,10 +16489,10 @@
                   <c:v>0.0650963405652961</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>0.0646085356872474</c:v>
+                  <c:v>0.0646085356872473</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>0.0641207308091986</c:v>
+                  <c:v>0.0641207308091985</c:v>
                 </c:pt>
                 <c:pt idx="217">
                   <c:v>0.0636329259311498</c:v>
@@ -16501,10 +16504,10 @@
                   <c:v>0.0626573161750522</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>0.0621695112970035</c:v>
+                  <c:v>0.0621695112970034</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>0.0616817064189547</c:v>
+                  <c:v>0.0616817064189546</c:v>
                 </c:pt>
                 <c:pt idx="222">
                   <c:v>0.0611939015409059</c:v>
@@ -16516,10 +16519,10 @@
                   <c:v>0.0602182917848083</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>0.0597304869067596</c:v>
+                  <c:v>0.0597304869067595</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>0.0592426820287108</c:v>
+                  <c:v>0.0592426820287107</c:v>
                 </c:pt>
                 <c:pt idx="227">
                   <c:v>0.058754877150662</c:v>
@@ -16534,7 +16537,7 @@
                   <c:v>0.0572914625165156</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>0.0568036576384669</c:v>
+                  <c:v>0.0568036576384668</c:v>
                 </c:pt>
                 <c:pt idx="232">
                   <c:v>0.0563158527604181</c:v>
@@ -16549,10 +16552,10 @@
                   <c:v>0.0548524381262717</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>0.054364633248223</c:v>
+                  <c:v>0.0543646332482229</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>0.0538768283701742</c:v>
+                  <c:v>0.0538768283701741</c:v>
                 </c:pt>
                 <c:pt idx="238">
                   <c:v>0.0533890234921254</c:v>
@@ -16564,10 +16567,10 @@
                   <c:v>0.0524134137360278</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>0.0519256088579791</c:v>
+                  <c:v>0.051925608857979</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>0.0514378039799303</c:v>
+                  <c:v>0.0514378039799302</c:v>
                 </c:pt>
                 <c:pt idx="243">
                   <c:v>0.0509499991018815</c:v>
@@ -16579,10 +16582,10 @@
                   <c:v>0.0499743893457839</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>0.0494865844677352</c:v>
+                  <c:v>0.0494865844677351</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>0.0489987795896864</c:v>
+                  <c:v>0.0489987795896863</c:v>
                 </c:pt>
                 <c:pt idx="248">
                   <c:v>0.0485109747116376</c:v>
@@ -16594,10 +16597,10 @@
                   <c:v>0.04753536495554</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>0.0470475600774913</c:v>
+                  <c:v>0.0470475600774912</c:v>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>0.0465597551994425</c:v>
+                  <c:v>0.0465597551994424</c:v>
                 </c:pt>
                 <c:pt idx="253">
                   <c:v>0.0460719503213937</c:v>
@@ -16609,13 +16612,13 @@
                   <c:v>0.0450963405652961</c:v>
                 </c:pt>
                 <c:pt idx="256">
-                  <c:v>0.0446085356872474</c:v>
+                  <c:v>0.0446085356872473</c:v>
                 </c:pt>
                 <c:pt idx="257">
-                  <c:v>0.0441207308091986</c:v>
+                  <c:v>0.0441207308091985</c:v>
                 </c:pt>
                 <c:pt idx="258">
-                  <c:v>0.0436329259311498</c:v>
+                  <c:v>0.0436329259311497</c:v>
                 </c:pt>
                 <c:pt idx="259">
                   <c:v>0.043145121053101</c:v>
@@ -21130,11 +21133,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="8419438"/>
-        <c:axId val="32761650"/>
+        <c:axId val="51981376"/>
+        <c:axId val="96828614"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="8419438"/>
+        <c:axId val="51981376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21166,14 +21169,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32761650"/>
+        <c:crossAx val="96828614"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32761650"/>
+        <c:axId val="96828614"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21215,7 +21218,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8419438"/>
+        <c:crossAx val="51981376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -21279,7 +21282,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart52.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -21290,10 +21293,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0464930500079885"/>
-          <c:y val="0.0268163496452247"/>
-          <c:w val="0.940933056398786"/>
-          <c:h val="0.59105899596922"/>
+          <c:x val="0.0464941822418719"/>
+          <c:y val="0.0268172429875408"/>
+          <c:w val="0.940912645842976"/>
+          <c:h val="0.591045372776334"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -41614,11 +41617,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="1190123"/>
-        <c:axId val="78832038"/>
+        <c:axId val="41632369"/>
+        <c:axId val="9938741"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1190123"/>
+        <c:axId val="41632369"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -41650,14 +41653,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78832038"/>
+        <c:crossAx val="9938741"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78832038"/>
+        <c:axId val="9938741"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -41700,7 +41703,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1190123"/>
+        <c:crossAx val="41632369"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -41775,9 +41778,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>83</xdr:col>
-      <xdr:colOff>100440</xdr:colOff>
+      <xdr:colOff>100080</xdr:colOff>
       <xdr:row>85</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -41785,8 +41788,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="29330280" y="2223000"/>
-        <a:ext cx="22582800" cy="10793160"/>
+        <a:off x="29359440" y="2223000"/>
+        <a:ext cx="22605480" cy="10792800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -41805,9 +41808,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>83</xdr:col>
-      <xdr:colOff>62280</xdr:colOff>
+      <xdr:colOff>61920</xdr:colOff>
       <xdr:row>156</xdr:row>
-      <xdr:rowOff>24120</xdr:rowOff>
+      <xdr:rowOff>23760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -41815,8 +41818,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="29342880" y="12992040"/>
-        <a:ext cx="22532040" cy="10806480"/>
+        <a:off x="29372040" y="12992040"/>
+        <a:ext cx="22554720" cy="10806120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -41835,9 +41838,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>303480</xdr:colOff>
+      <xdr:colOff>303120</xdr:colOff>
       <xdr:row>182</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -41848,8 +41851,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14947200" y="27645840"/>
-          <a:ext cx="303480" cy="303480"/>
+          <a:off x="14961600" y="27645840"/>
+          <a:ext cx="303120" cy="303120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -41877,9 +41880,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>621000</xdr:colOff>
+      <xdr:colOff>620640</xdr:colOff>
       <xdr:row>182</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -41890,8 +41893,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15264720" y="27645840"/>
-          <a:ext cx="303480" cy="303480"/>
+          <a:off x="15279120" y="27645840"/>
+          <a:ext cx="303120" cy="303120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -41919,9 +41922,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>265680</xdr:colOff>
+      <xdr:colOff>265320</xdr:colOff>
       <xdr:row>182</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -41932,8 +41935,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15584400" y="27645840"/>
-          <a:ext cx="253080" cy="303480"/>
+          <a:off x="15599880" y="27645840"/>
+          <a:ext cx="252720" cy="303120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -41962,11 +41965,11 @@
   </sheetPr>
   <dimension ref="A1:BL284"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A238" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J285" activeCellId="0" sqref="J285"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AV248" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BB274" activeCellId="0" sqref="BB274"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.16"/>
   </cols>
@@ -56088,6 +56091,10 @@
         <f aca="false">J185+$AD$175</f>
         <v>0.206571095983571</v>
       </c>
+      <c r="R186" s="1" t="n">
+        <f aca="false">Q189+R189+S189+P189+L189</f>
+        <v>1.00000000001714</v>
+      </c>
       <c r="Z186" s="4" t="n">
         <f aca="false">(P271-P189)/(ROW(P271)-ROW(P189))</f>
         <v>0.000121951219512195</v>
@@ -56488,7 +56495,7 @@
       </c>
       <c r="V190" s="4" t="n">
         <f aca="false">V189+$AF$186</f>
-        <v>0.0802182917848084</v>
+        <v>0.0802182917848083</v>
       </c>
       <c r="W190" s="4" t="n">
         <f aca="false">W189+$AG$186</f>
@@ -56616,7 +56623,7 @@
       </c>
       <c r="V191" s="4" t="n">
         <f aca="false">V190+$AF$186</f>
-        <v>0.0797304869067596</v>
+        <v>0.0797304869067595</v>
       </c>
       <c r="W191" s="4" t="n">
         <f aca="false">W190+$AG$186</f>
@@ -57256,7 +57263,7 @@
       </c>
       <c r="V196" s="4" t="n">
         <f aca="false">V195+$AF$186</f>
-        <v>0.0772914625165157</v>
+        <v>0.0772914625165156</v>
       </c>
       <c r="W196" s="4" t="n">
         <f aca="false">W195+$AG$186</f>
@@ -57896,7 +57903,7 @@
       </c>
       <c r="V201" s="4" t="n">
         <f aca="false">V200+$AF$186</f>
-        <v>0.0748524381262718</v>
+        <v>0.0748524381262717</v>
       </c>
       <c r="W201" s="4" t="n">
         <f aca="false">W200+$AG$186</f>
@@ -58024,7 +58031,7 @@
       </c>
       <c r="V202" s="4" t="n">
         <f aca="false">V201+$AF$186</f>
-        <v>0.074364633248223</v>
+        <v>0.0743646332482229</v>
       </c>
       <c r="W202" s="4" t="n">
         <f aca="false">W201+$AG$186</f>
@@ -58536,7 +58543,7 @@
       </c>
       <c r="V206" s="4" t="n">
         <f aca="false">V205+$AF$186</f>
-        <v>0.0724134137360279</v>
+        <v>0.0724134137360278</v>
       </c>
       <c r="W206" s="4" t="n">
         <f aca="false">W205+$AG$186</f>
@@ -58664,7 +58671,7 @@
       </c>
       <c r="V207" s="4" t="n">
         <f aca="false">V206+$AF$186</f>
-        <v>0.0719256088579791</v>
+        <v>0.071925608857979</v>
       </c>
       <c r="W207" s="4" t="n">
         <f aca="false">W206+$AG$186</f>
@@ -59176,7 +59183,7 @@
       </c>
       <c r="V211" s="4" t="n">
         <f aca="false">V210+$AF$186</f>
-        <v>0.069974389345784</v>
+        <v>0.0699743893457839</v>
       </c>
       <c r="W211" s="4" t="n">
         <f aca="false">W210+$AG$186</f>
@@ -59304,7 +59311,7 @@
       </c>
       <c r="V212" s="4" t="n">
         <f aca="false">V211+$AF$186</f>
-        <v>0.0694865844677352</v>
+        <v>0.0694865844677351</v>
       </c>
       <c r="W212" s="4" t="n">
         <f aca="false">W211+$AG$186</f>
@@ -59944,7 +59951,7 @@
       </c>
       <c r="V217" s="4" t="n">
         <f aca="false">V216+$AF$186</f>
-        <v>0.0670475600774913</v>
+        <v>0.0670475600774912</v>
       </c>
       <c r="W217" s="4" t="n">
         <f aca="false">W216+$AG$186</f>
@@ -60584,7 +60591,7 @@
       </c>
       <c r="V222" s="4" t="n">
         <f aca="false">V221+$AF$186</f>
-        <v>0.0646085356872474</v>
+        <v>0.0646085356872473</v>
       </c>
       <c r="W222" s="4" t="n">
         <f aca="false">W221+$AG$186</f>
@@ -60712,7 +60719,7 @@
       </c>
       <c r="V223" s="4" t="n">
         <f aca="false">V222+$AF$186</f>
-        <v>0.0641207308091986</v>
+        <v>0.0641207308091985</v>
       </c>
       <c r="W223" s="4" t="n">
         <f aca="false">W222+$AG$186</f>
@@ -61224,7 +61231,7 @@
       </c>
       <c r="V227" s="4" t="n">
         <f aca="false">V226+$AF$186</f>
-        <v>0.0621695112970035</v>
+        <v>0.0621695112970034</v>
       </c>
       <c r="W227" s="4" t="n">
         <f aca="false">W226+$AG$186</f>
@@ -61352,7 +61359,7 @@
       </c>
       <c r="V228" s="4" t="n">
         <f aca="false">V227+$AF$186</f>
-        <v>0.0616817064189547</v>
+        <v>0.0616817064189546</v>
       </c>
       <c r="W228" s="4" t="n">
         <f aca="false">W227+$AG$186</f>
@@ -61864,7 +61871,7 @@
       </c>
       <c r="V232" s="4" t="n">
         <f aca="false">V231+$AF$186</f>
-        <v>0.0597304869067596</v>
+        <v>0.0597304869067595</v>
       </c>
       <c r="W232" s="4" t="n">
         <f aca="false">W231+$AG$186</f>
@@ -61992,7 +61999,7 @@
       </c>
       <c r="V233" s="4" t="n">
         <f aca="false">V232+$AF$186</f>
-        <v>0.0592426820287108</v>
+        <v>0.0592426820287107</v>
       </c>
       <c r="W233" s="4" t="n">
         <f aca="false">W232+$AG$186</f>
@@ -62632,7 +62639,7 @@
       </c>
       <c r="V238" s="4" t="n">
         <f aca="false">V237+$AF$186</f>
-        <v>0.0568036576384669</v>
+        <v>0.0568036576384668</v>
       </c>
       <c r="W238" s="4" t="n">
         <f aca="false">W237+$AG$186</f>
@@ -63272,7 +63279,7 @@
       </c>
       <c r="V243" s="4" t="n">
         <f aca="false">V242+$AF$186</f>
-        <v>0.054364633248223</v>
+        <v>0.0543646332482229</v>
       </c>
       <c r="W243" s="4" t="n">
         <f aca="false">W242+$AG$186</f>
@@ -63400,7 +63407,7 @@
       </c>
       <c r="V244" s="4" t="n">
         <f aca="false">V243+$AF$186</f>
-        <v>0.0538768283701742</v>
+        <v>0.0538768283701741</v>
       </c>
       <c r="W244" s="4" t="n">
         <f aca="false">W243+$AG$186</f>
@@ -63912,7 +63919,7 @@
       </c>
       <c r="V248" s="4" t="n">
         <f aca="false">V247+$AF$186</f>
-        <v>0.0519256088579791</v>
+        <v>0.051925608857979</v>
       </c>
       <c r="W248" s="4" t="n">
         <f aca="false">W247+$AG$186</f>
@@ -64040,7 +64047,7 @@
       </c>
       <c r="V249" s="4" t="n">
         <f aca="false">V248+$AF$186</f>
-        <v>0.0514378039799303</v>
+        <v>0.0514378039799302</v>
       </c>
       <c r="W249" s="4" t="n">
         <f aca="false">W248+$AG$186</f>
@@ -64552,7 +64559,7 @@
       </c>
       <c r="V253" s="4" t="n">
         <f aca="false">V252+$AF$186</f>
-        <v>0.0494865844677352</v>
+        <v>0.0494865844677351</v>
       </c>
       <c r="W253" s="4" t="n">
         <f aca="false">W252+$AG$186</f>
@@ -64680,7 +64687,7 @@
       </c>
       <c r="V254" s="4" t="n">
         <f aca="false">V253+$AF$186</f>
-        <v>0.0489987795896864</v>
+        <v>0.0489987795896863</v>
       </c>
       <c r="W254" s="4" t="n">
         <f aca="false">W253+$AG$186</f>
@@ -65192,7 +65199,7 @@
       </c>
       <c r="V258" s="4" t="n">
         <f aca="false">V257+$AF$186</f>
-        <v>0.0470475600774913</v>
+        <v>0.0470475600774912</v>
       </c>
       <c r="W258" s="4" t="n">
         <f aca="false">W257+$AG$186</f>
@@ -65320,7 +65327,7 @@
       </c>
       <c r="V259" s="4" t="n">
         <f aca="false">V258+$AF$186</f>
-        <v>0.0465597551994425</v>
+        <v>0.0465597551994424</v>
       </c>
       <c r="W259" s="4" t="n">
         <f aca="false">W258+$AG$186</f>
@@ -65832,7 +65839,7 @@
       </c>
       <c r="V263" s="4" t="n">
         <f aca="false">V262+$AF$186</f>
-        <v>0.0446085356872474</v>
+        <v>0.0446085356872473</v>
       </c>
       <c r="W263" s="4" t="n">
         <f aca="false">W262+$AG$186</f>
@@ -65960,7 +65967,7 @@
       </c>
       <c r="V264" s="4" t="n">
         <f aca="false">V263+$AF$186</f>
-        <v>0.0441207308091986</v>
+        <v>0.0441207308091985</v>
       </c>
       <c r="W264" s="4" t="n">
         <f aca="false">W263+$AG$186</f>
@@ -66088,7 +66095,7 @@
       </c>
       <c r="V265" s="4" t="n">
         <f aca="false">V264+$AF$186</f>
-        <v>0.0436329259311498</v>
+        <v>0.0436329259311497</v>
       </c>
       <c r="W265" s="4" t="n">
         <f aca="false">W264+$AG$186</f>
@@ -66600,7 +66607,7 @@
       </c>
       <c r="V269" s="4" t="n">
         <f aca="false">V268+$AF$186</f>
-        <v>0.0416817064189547</v>
+        <v>0.0416817064189546</v>
       </c>
       <c r="W269" s="4" t="n">
         <f aca="false">W268+$AG$186</f>
@@ -66728,7 +66735,7 @@
       </c>
       <c r="V270" s="4" t="n">
         <f aca="false">V269+$AF$186</f>
-        <v>0.0411939015409059</v>
+        <v>0.0411939015409058</v>
       </c>
       <c r="W270" s="4" t="n">
         <f aca="false">W269+$AG$186</f>
@@ -67036,6 +67043,10 @@
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R278" s="1" t="n">
+        <f aca="false">P271+Q271+R271+S271+L271</f>
+        <v>1.00000000001714</v>
+      </c>
       <c r="AZ278" s="1"/>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Start simulation with possible semestral mobility, labour-market data up to second quarter of 2020; correct error with cal_est_m_p csv files.
</commit_message>
<xml_diff>
--- a/Excel_files_for_MISSAR/Prospective_scenarios/2014_q4_start/Historical_graphs_ages_16_69/Economic_scenarios_representation_dec_2019.xlsx
+++ b/Excel_files_for_MISSAR/Prospective_scenarios/2014_q4_start/Historical_graphs_ages_16_69/Economic_scenarios_representation_dec_2019.xlsx
@@ -836,7 +836,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart83.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -847,10 +847,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0524911879584643"/>
-          <c:y val="0.0202808632709563"/>
-          <c:w val="0.917436727954019"/>
-          <c:h val="0.625571233196571"/>
+          <c:x val="0.0524822919802875"/>
+          <c:y val="0.0202822163658805"/>
+          <c:w val="0.917410112982712"/>
+          <c:h val="0.62554625212663"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2029,6 +2029,12 @@
                 </c:pt>
                 <c:pt idx="180">
                   <c:v>0.3570887033</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.3600888513</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.36531013964385</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6521,6 +6527,12 @@
                 <c:pt idx="180">
                   <c:v>0.067043788</c:v>
                 </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.06689386</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.065</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8807,6 +8819,12 @@
                 <c:pt idx="180">
                   <c:v>0.2888602205</c:v>
                 </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.2715231188</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.18245591793928</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -13294,6 +13312,12 @@
                 </c:pt>
                 <c:pt idx="180">
                   <c:v>0.0659817544</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.0761241623</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.08480992921843</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17791,6 +17815,12 @@
                 <c:pt idx="180">
                   <c:v>0.2210255338</c:v>
                 </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.2253700076</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.30242401319844</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -21113,11 +21143,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="77694796"/>
-        <c:axId val="66511505"/>
+        <c:axId val="78890085"/>
+        <c:axId val="77709923"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77694796"/>
+        <c:axId val="78890085"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21149,14 +21179,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66511505"/>
+        <c:crossAx val="77709923"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66511505"/>
+        <c:axId val="77709923"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21198,7 +21228,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77694796"/>
+        <c:crossAx val="78890085"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -21262,7 +21292,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart84.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -21273,10 +21303,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0464983052465747"/>
-          <c:y val="0.0268190298507463"/>
-          <c:w val="0.940882544835378"/>
-          <c:h val="0.591018123667377"/>
+          <c:x val="0.0465012864085379"/>
+          <c:y val="0.026820816952089"/>
+          <c:w val="0.940841088841597"/>
+          <c:h val="0.590990870926901"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -22459,6 +22489,12 @@
                 <c:pt idx="180">
                   <c:v>0.2685366332</c:v>
                 </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.2655509646</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.2724304143814</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -26959,6 +26995,12 @@
                 <c:pt idx="180">
                   <c:v>0.0439037474</c:v>
                 </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.0372234087</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.04</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -29248,6 +29290,12 @@
                 <c:pt idx="180">
                   <c:v>0.2132496646</c:v>
                 </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.2092353789</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.12996209263928</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -33745,6 +33793,12 @@
                 <c:pt idx="180">
                   <c:v>0.0558333711</c:v>
                 </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.0658086325</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.066019220124</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -38242,6 +38296,12 @@
                 <c:pt idx="180">
                   <c:v>0.4184765837</c:v>
                 </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.4221816153</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.49158827285532</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -41573,11 +41633,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="82715660"/>
-        <c:axId val="54185967"/>
+        <c:axId val="16357236"/>
+        <c:axId val="86792990"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82715660"/>
+        <c:axId val="16357236"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -41609,14 +41669,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54185967"/>
+        <c:crossAx val="86792990"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54185967"/>
+        <c:axId val="86792990"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -41659,7 +41719,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82715660"/>
+        <c:crossAx val="16357236"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -41734,9 +41794,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>83</xdr:col>
-      <xdr:colOff>99360</xdr:colOff>
+      <xdr:colOff>98640</xdr:colOff>
       <xdr:row>85</xdr:row>
-      <xdr:rowOff>61560</xdr:rowOff>
+      <xdr:rowOff>60840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -41744,8 +41804,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="29447280" y="2223360"/>
-        <a:ext cx="22673160" cy="10792080"/>
+        <a:off x="29505600" y="2223360"/>
+        <a:ext cx="22718160" cy="10791360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -41764,9 +41824,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>80</xdr:col>
-      <xdr:colOff>333720</xdr:colOff>
+      <xdr:colOff>333000</xdr:colOff>
       <xdr:row>152</xdr:row>
-      <xdr:rowOff>23040</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -41774,8 +41834,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="27849960" y="12382200"/>
-        <a:ext cx="22622400" cy="10805400"/>
+        <a:off x="27904680" y="12382200"/>
+        <a:ext cx="22667400" cy="10804680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -41794,9 +41854,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>302400</xdr:colOff>
+      <xdr:colOff>301680</xdr:colOff>
       <xdr:row>182</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -41807,8 +41867,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15005520" y="27656280"/>
-          <a:ext cx="302400" cy="302400"/>
+          <a:off x="15034680" y="27656280"/>
+          <a:ext cx="301680" cy="301680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -41836,9 +41896,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>619920</xdr:colOff>
+      <xdr:colOff>619200</xdr:colOff>
       <xdr:row>182</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -41849,8 +41909,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15323040" y="27656280"/>
-          <a:ext cx="302400" cy="302400"/>
+          <a:off x="15352200" y="27656280"/>
+          <a:ext cx="301680" cy="301680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -41878,9 +41938,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>264600</xdr:colOff>
+      <xdr:colOff>263880</xdr:colOff>
       <xdr:row>182</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -41891,8 +41951,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15645600" y="27656280"/>
-          <a:ext cx="252000" cy="302400"/>
+          <a:off x="15675840" y="27656280"/>
+          <a:ext cx="251280" cy="301680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -41921,11 +41981,11 @@
   </sheetPr>
   <dimension ref="A1:BL284"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AK250" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AT271" activeCellId="0" sqref="AT271"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AM176" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AS180" activeCellId="0" sqref="AS180"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.16"/>
   </cols>
@@ -56211,6 +56271,21 @@
         <f aca="false">E184+1</f>
         <v>2020</v>
       </c>
+      <c r="F188" s="1" t="n">
+        <v>0.3600888513</v>
+      </c>
+      <c r="G188" s="1" t="n">
+        <v>0.06689386</v>
+      </c>
+      <c r="H188" s="1" t="n">
+        <v>0.2715231188</v>
+      </c>
+      <c r="I188" s="1" t="n">
+        <v>0.0761241623</v>
+      </c>
+      <c r="J188" s="1" t="n">
+        <v>0.2253700076</v>
+      </c>
       <c r="K188" s="5" t="n">
         <f aca="false">F187</f>
         <v>0.3570887033</v>
@@ -56238,6 +56313,21 @@
       <c r="AJ188" s="0" t="n">
         <f aca="false">AJ184+1</f>
         <v>2020</v>
+      </c>
+      <c r="AK188" s="1" t="n">
+        <v>0.2655509646</v>
+      </c>
+      <c r="AL188" s="1" t="n">
+        <v>0.0372234087</v>
+      </c>
+      <c r="AM188" s="1" t="n">
+        <v>0.2092353789</v>
+      </c>
+      <c r="AN188" s="1" t="n">
+        <v>0.0658086325</v>
+      </c>
+      <c r="AO188" s="1" t="n">
+        <v>0.4221816153</v>
       </c>
       <c r="AP188" s="5" t="n">
         <f aca="false">AK187</f>
@@ -56274,6 +56364,25 @@
         <f aca="false">E185+1</f>
         <v>2020</v>
       </c>
+      <c r="F189" s="1" t="n">
+        <f aca="false">F188*1.0145</f>
+        <v>0.36531013964385</v>
+      </c>
+      <c r="G189" s="1" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="H189" s="1" t="n">
+        <f aca="false">1-(F189+G189+J189+I189)</f>
+        <v>0.18245591793928</v>
+      </c>
+      <c r="I189" s="1" t="n">
+        <f aca="false">I188*1.1141</f>
+        <v>0.08480992921843</v>
+      </c>
+      <c r="J189" s="1" t="n">
+        <f aca="false">J188*1.3419</f>
+        <v>0.30242401319844</v>
+      </c>
       <c r="K189" s="8" t="n">
         <v>0.345</v>
       </c>
@@ -56298,6 +56407,25 @@
       <c r="AJ189" s="0" t="n">
         <f aca="false">AJ185+1</f>
         <v>2020</v>
+      </c>
+      <c r="AK189" s="1" t="n">
+        <f aca="false">AK187*1.0145</f>
+        <v>0.2724304143814</v>
+      </c>
+      <c r="AL189" s="1" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="AM189" s="1" t="n">
+        <f aca="false">1-(AK189+AL189+AO189+AN189)</f>
+        <v>0.12996209263928</v>
+      </c>
+      <c r="AN189" s="1" t="n">
+        <f aca="false">AN188*1.0032</f>
+        <v>0.066019220124</v>
+      </c>
+      <c r="AO189" s="1" t="n">
+        <f aca="false">AO188*1.1644</f>
+        <v>0.49158827285532</v>
       </c>
       <c r="AP189" s="9" t="n">
         <v>0.26</v>
@@ -57091,7 +57219,7 @@
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B196" s="1" t="n">
         <f aca="false">K192-AP192</f>
-        <v>0.0883051565197531</v>
+        <v>0.0883051565197533</v>
       </c>
       <c r="E196" s="0" t="n">
         <f aca="false">E192+1</f>
@@ -57219,7 +57347,7 @@
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B197" s="1" t="n">
         <f aca="false">K193-AP193</f>
-        <v>0.0881816997296296</v>
+        <v>0.0881816997296299</v>
       </c>
       <c r="E197" s="0" t="n">
         <f aca="false">E193+1</f>
@@ -57347,7 +57475,7 @@
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B198" s="1" t="n">
         <f aca="false">K194-AP194</f>
-        <v>0.0880582429395061</v>
+        <v>0.0880582429395065</v>
       </c>
       <c r="E198" s="0" t="n">
         <f aca="false">E194+1</f>
@@ -57475,7 +57603,7 @@
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B199" s="1" t="n">
         <f aca="false">K195-AP195</f>
-        <v>0.0879347861493826</v>
+        <v>0.0879347861493822</v>
       </c>
       <c r="E199" s="0" t="n">
         <f aca="false">E195+1</f>
@@ -57603,7 +57731,7 @@
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B200" s="1" t="n">
         <f aca="false">K196-AP196</f>
-        <v>0.0878113293592591</v>
+        <v>0.0878113293592588</v>
       </c>
       <c r="E200" s="0" t="n">
         <f aca="false">E196+1</f>
@@ -57731,7 +57859,7 @@
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B201" s="1" t="n">
         <f aca="false">K197-AP197</f>
-        <v>0.0876878725691356</v>
+        <v>0.0876878725691354</v>
       </c>
       <c r="E201" s="0" t="n">
         <f aca="false">E197+1</f>
@@ -57859,7 +57987,7 @@
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B202" s="1" t="n">
         <f aca="false">K198-AP198</f>
-        <v>0.0875644157790121</v>
+        <v>0.087564415779012</v>
       </c>
       <c r="E202" s="0" t="n">
         <f aca="false">E198+1</f>
@@ -58115,7 +58243,7 @@
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B204" s="1" t="n">
         <f aca="false">K200-AP200</f>
-        <v>0.0873175021987652</v>
+        <v>0.0873175021987653</v>
       </c>
       <c r="E204" s="0" t="n">
         <f aca="false">E200+1</f>
@@ -58243,7 +58371,7 @@
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B205" s="1" t="n">
         <f aca="false">K201-AP201</f>
-        <v>0.0871940454086417</v>
+        <v>0.087194045408642</v>
       </c>
       <c r="E205" s="0" t="n">
         <f aca="false">E201+1</f>
@@ -58371,7 +58499,7 @@
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B206" s="1" t="n">
         <f aca="false">K202-AP202</f>
-        <v>0.0870705886185182</v>
+        <v>0.0870705886185186</v>
       </c>
       <c r="E206" s="0" t="n">
         <f aca="false">E202+1</f>
@@ -58499,7 +58627,7 @@
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B207" s="1" t="n">
         <f aca="false">K203-AP203</f>
-        <v>0.0869471318283947</v>
+        <v>0.0869471318283952</v>
       </c>
       <c r="E207" s="0" t="n">
         <f aca="false">E203+1</f>
@@ -58627,7 +58755,7 @@
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B208" s="1" t="n">
         <f aca="false">K204-AP204</f>
-        <v>0.0868236750382712</v>
+        <v>0.0868236750382708</v>
       </c>
       <c r="E208" s="0" t="n">
         <f aca="false">E204+1</f>
@@ -58755,7 +58883,7 @@
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B209" s="1" t="n">
         <f aca="false">K205-AP205</f>
-        <v>0.0867002182481477</v>
+        <v>0.0867002182481475</v>
       </c>
       <c r="E209" s="0" t="n">
         <f aca="false">E205+1</f>
@@ -58883,7 +59011,7 @@
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B210" s="1" t="n">
         <f aca="false">K206-AP206</f>
-        <v>0.0865767614580242</v>
+        <v>0.0865767614580241</v>
       </c>
       <c r="E210" s="0" t="n">
         <f aca="false">E206+1</f>
@@ -59139,7 +59267,7 @@
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B212" s="1" t="n">
         <f aca="false">K208-AP208</f>
-        <v>0.0863298478777773</v>
+        <v>0.0863298478777774</v>
       </c>
       <c r="E212" s="0" t="n">
         <f aca="false">E208+1</f>
@@ -59267,7 +59395,7 @@
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B213" s="1" t="n">
         <f aca="false">K209-AP209</f>
-        <v>0.0862063910876538</v>
+        <v>0.086206391087654</v>
       </c>
       <c r="E213" s="0" t="n">
         <f aca="false">E209+1</f>
@@ -59395,7 +59523,7 @@
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B214" s="1" t="n">
         <f aca="false">K210-AP210</f>
-        <v>0.0860829342975303</v>
+        <v>0.0860829342975306</v>
       </c>
       <c r="E214" s="0" t="n">
         <f aca="false">E210+1</f>
@@ -59523,7 +59651,7 @@
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B215" s="1" t="n">
         <f aca="false">K211-AP211</f>
-        <v>0.0859594775074068</v>
+        <v>0.0859594775074072</v>
       </c>
       <c r="E215" s="0" t="n">
         <f aca="false">E211+1</f>
@@ -59651,7 +59779,7 @@
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B216" s="1" t="n">
         <f aca="false">K212-AP212</f>
-        <v>0.0858360207172833</v>
+        <v>0.0858360207172829</v>
       </c>
       <c r="E216" s="0" t="n">
         <f aca="false">E212+1</f>
@@ -59779,7 +59907,7 @@
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B217" s="1" t="n">
         <f aca="false">K213-AP213</f>
-        <v>0.0857125639271598</v>
+        <v>0.0857125639271595</v>
       </c>
       <c r="E217" s="0" t="n">
         <f aca="false">E213+1</f>
@@ -59907,7 +60035,7 @@
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B218" s="1" t="n">
         <f aca="false">K214-AP214</f>
-        <v>0.0855891071370363</v>
+        <v>0.0855891071370361</v>
       </c>
       <c r="E218" s="0" t="n">
         <f aca="false">E214+1</f>
@@ -60291,7 +60419,7 @@
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B221" s="1" t="n">
         <f aca="false">K217-AP217</f>
-        <v>0.0852187367666659</v>
+        <v>0.085218736766666</v>
       </c>
       <c r="E221" s="0" t="n">
         <f aca="false">E217+1</f>
@@ -60419,7 +60547,7 @@
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B222" s="1" t="n">
         <f aca="false">K218-AP218</f>
-        <v>0.0850952799765424</v>
+        <v>0.0850952799765427</v>
       </c>
       <c r="E222" s="0" t="n">
         <f aca="false">E218+1</f>
@@ -60547,7 +60675,7 @@
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="1" t="n">
         <f aca="false">K219-AP219</f>
-        <v>0.0849718231864189</v>
+        <v>0.0849718231864193</v>
       </c>
       <c r="E223" s="0" t="n">
         <f aca="false">E219+1</f>
@@ -60675,7 +60803,7 @@
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="1" t="n">
         <f aca="false">K220-AP220</f>
-        <v>0.0848483663962954</v>
+        <v>0.0848483663962949</v>
       </c>
       <c r="E224" s="0" t="n">
         <f aca="false">E220+1</f>
@@ -60803,7 +60931,7 @@
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="1" t="n">
         <f aca="false">K221-AP221</f>
-        <v>0.0847249096061719</v>
+        <v>0.0847249096061715</v>
       </c>
       <c r="E225" s="0" t="n">
         <f aca="false">E221+1</f>
@@ -60931,7 +61059,7 @@
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="1" t="n">
         <f aca="false">K222-AP222</f>
-        <v>0.0846014528160484</v>
+        <v>0.0846014528160481</v>
       </c>
       <c r="E226" s="0" t="n">
         <f aca="false">E222+1</f>
@@ -61059,7 +61187,7 @@
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="1" t="n">
         <f aca="false">K223-AP223</f>
-        <v>0.0844779960259249</v>
+        <v>0.0844779960259248</v>
       </c>
       <c r="E227" s="0" t="n">
         <f aca="false">E223+1</f>
@@ -61315,7 +61443,7 @@
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B229" s="1" t="n">
         <f aca="false">K225-AP225</f>
-        <v>0.0842310824456779</v>
+        <v>0.0842310824456781</v>
       </c>
       <c r="E229" s="0" t="n">
         <f aca="false">E225+1</f>
@@ -61443,7 +61571,7 @@
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B230" s="1" t="n">
         <f aca="false">K226-AP226</f>
-        <v>0.0841076256555545</v>
+        <v>0.0841076256555547</v>
       </c>
       <c r="E230" s="0" t="n">
         <f aca="false">E226+1</f>
@@ -61571,7 +61699,7 @@
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="1" t="n">
         <f aca="false">K227-AP227</f>
-        <v>0.083984168865431</v>
+        <v>0.0839841688654313</v>
       </c>
       <c r="E231" s="0" t="n">
         <f aca="false">E227+1</f>
@@ -61699,7 +61827,7 @@
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="1" t="n">
         <f aca="false">K228-AP228</f>
-        <v>0.0838607120753075</v>
+        <v>0.0838607120753079</v>
       </c>
       <c r="E232" s="0" t="n">
         <f aca="false">E228+1</f>
@@ -61827,7 +61955,7 @@
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="1" t="n">
         <f aca="false">K229-AP229</f>
-        <v>0.083737255285184</v>
+        <v>0.0837372552851836</v>
       </c>
       <c r="E233" s="0" t="n">
         <f aca="false">E229+1</f>
@@ -61955,7 +62083,7 @@
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B234" s="1" t="n">
         <f aca="false">K230-AP230</f>
-        <v>0.0836137984950605</v>
+        <v>0.0836137984950602</v>
       </c>
       <c r="E234" s="0" t="n">
         <f aca="false">E230+1</f>
@@ -62083,7 +62211,7 @@
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B235" s="1" t="n">
         <f aca="false">K231-AP231</f>
-        <v>0.083490341704937</v>
+        <v>0.0834903417049368</v>
       </c>
       <c r="E235" s="0" t="n">
         <f aca="false">E231+1</f>
@@ -62339,7 +62467,7 @@
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B237" s="1" t="n">
         <f aca="false">K233-AP233</f>
-        <v>0.08324342812469</v>
+        <v>0.0832434281246901</v>
       </c>
       <c r="E237" s="0" t="n">
         <f aca="false">E233+1</f>
@@ -62467,7 +62595,7 @@
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="1" t="n">
         <f aca="false">K234-AP234</f>
-        <v>0.0831199713345666</v>
+        <v>0.0831199713345667</v>
       </c>
       <c r="E238" s="0" t="n">
         <f aca="false">E234+1</f>
@@ -62595,7 +62723,7 @@
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="1" t="n">
         <f aca="false">K235-AP235</f>
-        <v>0.0829965145444431</v>
+        <v>0.0829965145444433</v>
       </c>
       <c r="E239" s="0" t="n">
         <f aca="false">E235+1</f>
@@ -62723,7 +62851,7 @@
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B240" s="1" t="n">
         <f aca="false">K236-AP236</f>
-        <v>0.0828730577543196</v>
+        <v>0.08287305775432</v>
       </c>
       <c r="E240" s="0" t="n">
         <f aca="false">E236+1</f>
@@ -62851,7 +62979,7 @@
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="1" t="n">
         <f aca="false">K237-AP237</f>
-        <v>0.0827496009641961</v>
+        <v>0.0827496009641956</v>
       </c>
       <c r="E241" s="0" t="n">
         <f aca="false">E237+1</f>
@@ -62979,7 +63107,7 @@
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="1" t="n">
         <f aca="false">K238-AP238</f>
-        <v>0.0826261441740726</v>
+        <v>0.0826261441740722</v>
       </c>
       <c r="E242" s="0" t="n">
         <f aca="false">E238+1</f>
@@ -63107,7 +63235,7 @@
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="1" t="n">
         <f aca="false">K239-AP239</f>
-        <v>0.0825026873839491</v>
+        <v>0.0825026873839489</v>
       </c>
       <c r="E243" s="0" t="n">
         <f aca="false">E239+1</f>
@@ -63235,7 +63363,7 @@
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="1" t="n">
         <f aca="false">K240-AP240</f>
-        <v>0.0823792305938256</v>
+        <v>0.0823792305938255</v>
       </c>
       <c r="E244" s="0" t="n">
         <f aca="false">E240+1</f>
@@ -63491,7 +63619,7 @@
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B246" s="1" t="n">
         <f aca="false">K242-AP242</f>
-        <v>0.0821323170135786</v>
+        <v>0.0821323170135788</v>
       </c>
       <c r="E246" s="0" t="n">
         <f aca="false">E242+1</f>
@@ -63619,7 +63747,7 @@
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="1" t="n">
         <f aca="false">K243-AP243</f>
-        <v>0.0820088602234552</v>
+        <v>0.0820088602234554</v>
       </c>
       <c r="E247" s="0" t="n">
         <f aca="false">E243+1</f>
@@ -63747,7 +63875,7 @@
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="1" t="n">
         <f aca="false">K244-AP244</f>
-        <v>0.0818854034333317</v>
+        <v>0.081885403433332</v>
       </c>
       <c r="E248" s="0" t="n">
         <f aca="false">E244+1</f>
@@ -63875,7 +64003,7 @@
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="1" t="n">
         <f aca="false">K245-AP245</f>
-        <v>0.0817619466432082</v>
+        <v>0.0817619466432086</v>
       </c>
       <c r="E249" s="0" t="n">
         <f aca="false">E245+1</f>
@@ -64003,7 +64131,7 @@
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="1" t="n">
         <f aca="false">K246-AP246</f>
-        <v>0.0816384898530847</v>
+        <v>0.0816384898530843</v>
       </c>
       <c r="E250" s="0" t="n">
         <f aca="false">E246+1</f>
@@ -64131,7 +64259,7 @@
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="1" t="n">
         <f aca="false">K247-AP247</f>
-        <v>0.0815150330629612</v>
+        <v>0.0815150330629609</v>
       </c>
       <c r="E251" s="0" t="n">
         <f aca="false">E247+1</f>
@@ -64259,7 +64387,7 @@
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="1" t="n">
         <f aca="false">K248-AP248</f>
-        <v>0.0813915762728377</v>
+        <v>0.0813915762728376</v>
       </c>
       <c r="E252" s="0" t="n">
         <f aca="false">E248+1</f>
@@ -64515,7 +64643,7 @@
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="1" t="n">
         <f aca="false">K250-AP250</f>
-        <v>0.0811446626925907</v>
+        <v>0.0811446626925908</v>
       </c>
       <c r="E254" s="0" t="n">
         <f aca="false">E250+1</f>
@@ -64643,7 +64771,7 @@
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="1" t="n">
         <f aca="false">K251-AP251</f>
-        <v>0.0810212059024673</v>
+        <v>0.0810212059024674</v>
       </c>
       <c r="E255" s="0" t="n">
         <f aca="false">E251+1</f>
@@ -64771,7 +64899,7 @@
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="1" t="n">
         <f aca="false">K252-AP252</f>
-        <v>0.0808977491123438</v>
+        <v>0.080897749112344</v>
       </c>
       <c r="E256" s="0" t="n">
         <f aca="false">E252+1</f>
@@ -64899,7 +65027,7 @@
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="1" t="n">
         <f aca="false">K253-AP253</f>
-        <v>0.0807742923222203</v>
+        <v>0.0807742923222207</v>
       </c>
       <c r="E257" s="0" t="n">
         <f aca="false">E253+1</f>
@@ -65027,7 +65155,7 @@
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="1" t="n">
         <f aca="false">K254-AP254</f>
-        <v>0.0806508355320968</v>
+        <v>0.0806508355320963</v>
       </c>
       <c r="E258" s="0" t="n">
         <f aca="false">E254+1</f>
@@ -65155,7 +65283,7 @@
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="1" t="n">
         <f aca="false">K255-AP255</f>
-        <v>0.0805273787419733</v>
+        <v>0.080527378741973</v>
       </c>
       <c r="E259" s="0" t="n">
         <f aca="false">E255+1</f>
@@ -65283,7 +65411,7 @@
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="1" t="n">
         <f aca="false">K256-AP256</f>
-        <v>0.0804039219518498</v>
+        <v>0.0804039219518496</v>
       </c>
       <c r="E260" s="0" t="n">
         <f aca="false">E256+1</f>
@@ -65411,7 +65539,7 @@
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B261" s="1" t="n">
         <f aca="false">K257-AP257</f>
-        <v>0.0802804651617263</v>
+        <v>0.0802804651617262</v>
       </c>
       <c r="E261" s="0" t="n">
         <f aca="false">E257+1</f>
@@ -65667,7 +65795,7 @@
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B263" s="1" t="n">
         <f aca="false">K259-AP259</f>
-        <v>0.0800335515814794</v>
+        <v>0.0800335515814795</v>
       </c>
       <c r="E263" s="0" t="n">
         <f aca="false">E259+1</f>
@@ -65795,7 +65923,7 @@
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B264" s="1" t="n">
         <f aca="false">K260-AP260</f>
-        <v>0.0799100947913559</v>
+        <v>0.0799100947913561</v>
       </c>
       <c r="E264" s="0" t="n">
         <f aca="false">E260+1</f>
@@ -65923,7 +66051,7 @@
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B265" s="1" t="n">
         <f aca="false">K261-AP261</f>
-        <v>0.0797866380012324</v>
+        <v>0.0797866380012327</v>
       </c>
       <c r="E265" s="0" t="n">
         <f aca="false">E261+1</f>
@@ -66051,7 +66179,7 @@
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B266" s="1" t="n">
         <f aca="false">K262-AP262</f>
-        <v>0.0796631812111089</v>
+        <v>0.0796631812111094</v>
       </c>
       <c r="E266" s="0" t="n">
         <f aca="false">E262+1</f>
@@ -66179,7 +66307,7 @@
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B267" s="1" t="n">
         <f aca="false">K263-AP263</f>
-        <v>0.0795397244209854</v>
+        <v>0.079539724420985</v>
       </c>
       <c r="E267" s="0" t="n">
         <f aca="false">E263+1</f>
@@ -66307,7 +66435,7 @@
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B268" s="1" t="n">
         <f aca="false">K264-AP264</f>
-        <v>0.0794162676308619</v>
+        <v>0.0794162676308616</v>
       </c>
       <c r="E268" s="0" t="n">
         <f aca="false">E264+1</f>
@@ -66435,7 +66563,7 @@
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B269" s="1" t="n">
         <f aca="false">K265-AP265</f>
-        <v>0.0792928108407384</v>
+        <v>0.0792928108407383</v>
       </c>
       <c r="E269" s="0" t="n">
         <f aca="false">E265+1</f>

</xml_diff>